<commit_message>
ajout logique différence de restri
</commit_message>
<xml_diff>
--- a/Tili One Cup #3/compo.xlsx
+++ b/Tili One Cup #3/compo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joannes\Documents\Projects\Dofusdev\Tournaments-stats\Tiliwan_Cup#2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joannes\Documents\Projects\Dofusdev\Tournaments-stats\Tili One Cup #3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B890612-8309-4CB0-A496-AB5340E4FACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C695C036-4FB7-485A-BD22-6AFDA3937970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -167,12 +167,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -194,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -202,6 +208,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,7 +517,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,6 +600,7 @@
       <c r="D5" t="s">
         <v>20</v>
       </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -663,6 +671,7 @@
       <c r="D10" t="s">
         <v>13</v>
       </c>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -719,6 +728,7 @@
       <c r="D14" t="s">
         <v>20</v>
       </c>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -748,7 +758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -762,7 +772,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
@@ -776,7 +786,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -790,7 +800,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
@@ -804,7 +814,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>37</v>
       </c>
@@ -818,7 +828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>38</v>
       </c>
@@ -832,7 +842,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>39</v>
       </c>
@@ -846,7 +856,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
@@ -859,6 +869,7 @@
       <c r="D24" t="s">
         <v>5</v>
       </c>
+      <c r="E24" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>